<commit_message>
Se arreglan errores de consistencia en el codigo
</commit_message>
<xml_diff>
--- a/Codigo/src/principal/datos.xlsx
+++ b/Codigo/src/principal/datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeanSF\Documents\GitHub\Proyecto-Poo-1\Codigo\src\principal\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -150,12 +150,16 @@
   </si>
   <si>
     <t>Sin asignar</t>
+  </si>
+  <si>
+    <t>3.6 km norta de Carrizal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,9 +189,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
@@ -510,15 +515,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="3.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.97265625" collapsed="true" bestFit="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.71875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.71875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.38671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.28125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.8671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -954,6 +959,35 @@
       </c>
       <c r="I15">
         <v>9</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B16" t="n" s="2">
+        <v>42613.87513888889</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10.1187</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-84.161</v>
       </c>
     </row>
   </sheetData>
@@ -969,11 +1003,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.4296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.52734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambien el tamanno de una vetana : D
</commit_message>
<xml_diff>
--- a/Codigo/src/principal/datos.xlsx
+++ b/Codigo/src/principal/datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DeanSF\Documents\GitHub\Proyecto-Poo-1\Codigo\src\principal\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -153,12 +153,22 @@
   </si>
   <si>
     <t>Tectonico por falla local</t>
+  </si>
+  <si>
+    <t>Creado por angelo</t>
+  </si>
+  <si>
+    <t>Esteban Perez Picado</t>
+  </si>
+  <si>
+    <t>estebanPerezp2003@gmial.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,10 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -514,15 +525,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="3.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.97265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.71875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.30078125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.51953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.38671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.73828125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.41015625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -554,18 +565,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43831.042372685188</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B2" t="n" s="3">
+        <v>43831.04237268519</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.0</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -576,25 +587,25 @@
       <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="H2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n" s="3">
         <v>44185.847453703704</v>
       </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
+      <c r="C3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20.0</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -605,25 +616,25 @@
       <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="H3">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="H3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B4" t="n" s="3">
         <v>37683.127118055556</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>33</v>
+      <c r="C4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>33.0</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -634,25 +645,25 @@
       <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="H4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B5" t="n" s="3">
         <v>38081.169490740744</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
+      <c r="C5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.0</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -663,25 +674,25 @@
       <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="H5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B6" t="n" s="3">
         <v>38477.211863425924</v>
       </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
+      <c r="C6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5.0</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
@@ -692,25 +703,25 @@
       <c r="G6" t="s">
         <v>30</v>
       </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>38874.254236111112</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
+      <c r="H6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B7" t="n" s="3">
+        <v>38874.25423611111</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6.0</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -721,25 +732,25 @@
       <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="H7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B8" t="n" s="3">
         <v>39270.2966087963</v>
       </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
+      <c r="C8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7.0</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -750,25 +761,25 @@
       <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="H8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B9" t="n" s="3">
         <v>39302.33898148148</v>
       </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>8</v>
+      <c r="C9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8.0</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -779,25 +790,25 @@
       <c r="G9" t="s">
         <v>36</v>
       </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>40065.381354166668</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
+      <c r="H9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B10" t="n" s="3">
+        <v>40065.38135416667</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9.0</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -808,25 +819,25 @@
       <c r="G10" t="s">
         <v>39</v>
       </c>
-      <c r="H10">
-        <v>9</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
-        <v>40065.381354166668</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
+      <c r="H10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B11" t="n" s="3">
+        <v>40065.38135416667</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9.0</v>
       </c>
       <c r="E11" t="s">
         <v>37</v>
@@ -837,54 +848,54 @@
       <c r="G11" t="s">
         <v>39</v>
       </c>
-      <c r="H11">
-        <v>9</v>
-      </c>
-      <c r="I11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>40065.381354166668</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
+      <c r="H11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B12" t="n" s="3">
+        <v>42995.44809027778</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5200.0</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12">
-        <v>9</v>
-      </c>
-      <c r="I12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>40430.381354166668</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="H12" t="n">
+        <v>9.317183418558386</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-83.66737356962295</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B13" t="n" s="3">
+        <v>40430.38135416667</v>
+      </c>
+      <c r="C13" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9.0</v>
       </c>
       <c r="E13" t="s">
         <v>37</v>
@@ -895,25 +906,25 @@
       <c r="G13" t="s">
         <v>39</v>
       </c>
-      <c r="H13">
-        <v>9</v>
-      </c>
-      <c r="I13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="H13" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B14" t="n" s="3">
         <v>40826.423726851855</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
+      <c r="C14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>10.0</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -924,69 +935,98 @@
       <c r="G14" t="s">
         <v>40</v>
       </c>
-      <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44813.381354166668</v>
-      </c>
-      <c r="C15">
-        <v>99</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
+      <c r="H14" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B15" t="n" s="3">
+        <v>42613.87513888889</v>
+      </c>
+      <c r="C15" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>88.0</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15">
-        <v>9</v>
-      </c>
-      <c r="I15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>42613.875138888892</v>
-      </c>
-      <c r="C16">
-        <v>4.2</v>
-      </c>
-      <c r="D16">
-        <v>88</v>
+        <v>42</v>
+      </c>
+      <c r="H15" t="n">
+        <v>10.1187</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-84.161</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B16" t="n" s="3">
+        <v>42995.44809027778</v>
+      </c>
+      <c r="C16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5200.0</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
         <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16">
-        <v>10.1187</v>
-      </c>
-      <c r="I16">
-        <v>-84.161000000000001</v>
+        <v>44</v>
+      </c>
+      <c r="H16" t="n">
+        <v>9.317183418558386</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-83.66737356962295</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B17" t="n" s="3">
+        <v>42995.44809027778</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5200.0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="n">
+        <v>9.317183418558386</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-83.66737356962295</v>
       </c>
     </row>
   </sheetData>
@@ -996,17 +1036,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="45.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.07421875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.4296875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.99609375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.95703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1162,6 +1202,23 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2.08420336E8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6.1028259E7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambion el el grafico 5
Agregue y modifique algunos espacios
del JTable
</commit_message>
<xml_diff>
--- a/Codigo/src/principal/datos.xlsx
+++ b/Codigo/src/principal/datos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>17km Noroeste de Ciudad Cortes, Zona Sur</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -118,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -128,21 +132,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.859375" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.71875" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.30078125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.20703125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="39.4296875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.28125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.95703125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.97265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.71875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.30078125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.20703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="39.4296875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.27734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.94921875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -288,6 +292,35 @@
       </c>
       <c r="I5" t="n">
         <v>-83.669</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n" s="3">
+        <v>40461.423726851855</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -303,11 +336,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.39453125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.16015625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.29296875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.10546875" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.39453125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.16015625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.29296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.10546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>